<commit_message>
Add structure design partly and finish docs.xlsx.
</commit_message>
<xml_diff>
--- a/Notes/Docs.xlsx
+++ b/Notes/Docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PersonalFiles\Project\Kylin\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2474B30A-D564-48D8-BBFC-13511F82A2A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7475F468-C1C2-4FC0-937B-9A81BE5CECAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="27096" windowHeight="16416" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="27096" windowHeight="16416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -1523,7 +1523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="D3" sqref="D3"/>
     </sheetView>
@@ -2888,9 +2888,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A16F03-21AF-4C99-987E-D76AB0EA733D}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>